<commit_message>
[AA | 13/4/2018] : commit for Sample tab changes and profile page
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332BC8E9-3876-449D-B4FC-C7B056578CAE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7C7D1-C63A-40B1-AE3D-FC8E90B28C49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{9FF0C8AF-150F-44C8-9E9F-D2E2CBFEAF09}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{686FF519-5F74-41F7-8B20-DF3D6149B580}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Categorical_Data" sheetId="5" r:id="rId1"/>
+    <sheet name="Profile_Data" sheetId="4" r:id="rId2"/>
+    <sheet name="Sample_Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Fields_Data" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +29,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
   <si>
     <t>User</t>
   </si>
@@ -73,6 +104,60 @@
   </si>
   <si>
     <t>User48</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Scale Type</t>
+  </si>
+  <si>
+    <t>Distinct Count</t>
+  </si>
+  <si>
+    <t>Unique Count(%)</t>
+  </si>
+  <si>
+    <t>Missing(%)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>jobinstanceid</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -108,8 +193,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,13 +509,289 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63713B9-6357-4A72-9D8A-6B5260E8F81D}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258EB639-EA61-477D-98E2-6A869BB70443}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>777</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>666</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>555</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>444</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>333</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>222</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>200</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.1111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE145A48-B877-4FE4-AFD8-C169CA3698A6}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>90</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CCCAB-3C83-4826-8754-CDF22F24FE6F}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
@@ -438,13 +800,13 @@
         <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D1">
         <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F1">
         <v>10000</v>
@@ -458,13 +820,13 @@
         <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>20000</v>
@@ -478,13 +840,13 @@
         <v>500</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>40000</v>
@@ -498,13 +860,13 @@
         <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>60000</v>
@@ -518,13 +880,13 @@
         <v>333</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>70000</v>
@@ -538,13 +900,13 @@
         <v>444</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>90000</v>
@@ -558,13 +920,13 @@
         <v>555</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>120000</v>
@@ -578,13 +940,13 @@
         <v>666</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>230000</v>
@@ -598,13 +960,13 @@
         <v>777</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D9">
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>120000</v>
@@ -618,4 +980,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4354C65F-217B-4E18-B9F8-2FDD8991002A}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B04FFD-6DE8-406C-BAD2-FF88C9BE92CC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[AA | 16/04/2018] : Changes for Profile tab and Framework restruture
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7C7D1-C63A-40B1-AE3D-FC8E90B28C49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B66BE0-DD3C-483C-B90A-2B0FAE812014}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{686FF519-5F74-41F7-8B20-DF3D6149B580}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="1" activeTab="1" xr2:uid="{686FF519-5F74-41F7-8B20-DF3D6149B580}"/>
   </bookViews>
   <sheets>
-    <sheet name="Categorical_Data" sheetId="5" r:id="rId1"/>
-    <sheet name="Profile_Data" sheetId="4" r:id="rId2"/>
-    <sheet name="Sample_Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Fields_Data" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Visualize" sheetId="6" r:id="rId1"/>
+    <sheet name="DescriptiveStatistics_Data" sheetId="8" r:id="rId2"/>
+    <sheet name="QuantileStatistics_Data" sheetId="7" r:id="rId3"/>
+    <sheet name="Categorical_Data" sheetId="5" r:id="rId4"/>
+    <sheet name="Profile_Data" sheetId="4" r:id="rId5"/>
+    <sheet name="Sample_Data" sheetId="3" r:id="rId6"/>
+    <sheet name="Fields_Data" sheetId="2" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -158,6 +161,117 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>AAVESH</t>
+  </si>
+  <si>
+    <t>ANALYST</t>
+  </si>
+  <si>
+    <t>DALLAS</t>
+  </si>
+  <si>
+    <t>AMAN</t>
+  </si>
+  <si>
+    <t>PRESIDENT</t>
+  </si>
+  <si>
+    <t>SANTOSH</t>
+  </si>
+  <si>
+    <t>CLERK</t>
+  </si>
+  <si>
+    <t>CHICAGO</t>
+  </si>
+  <si>
+    <t>MILLER</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>SUYOG</t>
+  </si>
+  <si>
+    <t>SANGEETA</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t>GIRISH</t>
+  </si>
+  <si>
+    <t>AMOL</t>
+  </si>
+  <si>
+    <t>NISHA</t>
+  </si>
+  <si>
+    <t>MARTIN</t>
+  </si>
+  <si>
+    <t>SALESMAN</t>
+  </si>
+  <si>
+    <t>SCOTT</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>5-th Percentile</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>95-th Percentile</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Interquartile range</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Coef of variation</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Memory size</t>
   </si>
 </sst>
 </file>
@@ -193,9 +307,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +624,413 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A36E2ED-4772-47F9-B35C-8CB5C4409702}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2">
+        <v>29923</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2">
+        <v>31920</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="2">
+        <v>29923</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2">
+        <v>29974</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2">
+        <v>29746</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="2">
+        <v>29678</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2">
+        <v>29637</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2">
+        <v>29707</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="2">
+        <v>29907</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2">
+        <v>29857</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="2">
+        <v>31886</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="2">
+        <v>31886</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8818ED2-DC59-4EB8-A9A5-6F4594129690}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1">
+        <v>226.58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
+        <v>-1.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>421.89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>185.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8">
+        <v>51338.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9">
+        <v>3560</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA5F027-FF63-48EB-B373-A7B956E95C47}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>610.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>399.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258EB639-EA61-477D-98E2-6A869BB70443}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -631,7 +1149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE145A48-B877-4FE4-AFD8-C169CA3698A6}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -784,7 +1302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CCCAB-3C83-4826-8754-CDF22F24FE6F}">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -982,7 +1500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4354C65F-217B-4E18-B9F8-2FDD8991002A}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -1080,7 +1598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B04FFD-6DE8-406C-BAD2-FF88C9BE92CC}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
[ST 20 April 2018] - Updated code for developers tab
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_Local\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B66BE0-DD3C-483C-B90A-2B0FAE812014}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="1" activeTab="1" xr2:uid="{686FF519-5F74-41F7-8B20-DF3D6149B580}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Visualize" sheetId="6" r:id="rId1"/>
-    <sheet name="DescriptiveStatistics_Data" sheetId="8" r:id="rId2"/>
-    <sheet name="QuantileStatistics_Data" sheetId="7" r:id="rId3"/>
-    <sheet name="Categorical_Data" sheetId="5" r:id="rId4"/>
-    <sheet name="Profile_Data" sheetId="4" r:id="rId5"/>
-    <sheet name="Sample_Data" sheetId="3" r:id="rId6"/>
-    <sheet name="Fields_Data" sheetId="2" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
+    <sheet name="DeveloperTabData" sheetId="9" r:id="rId2"/>
+    <sheet name="DescriptiveStatistics_Data" sheetId="8" r:id="rId3"/>
+    <sheet name="QuantileStatistics_Data" sheetId="7" r:id="rId4"/>
+    <sheet name="Categorical_Data" sheetId="5" r:id="rId5"/>
+    <sheet name="Profile_Data" sheetId="4" r:id="rId6"/>
+    <sheet name="Sample_Data" sheetId="3" r:id="rId7"/>
+    <sheet name="Fields_Data" sheetId="2" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -272,12 +272,42 @@
   </si>
   <si>
     <t>Memory size</t>
+  </si>
+  <si>
+    <t>Shell Script</t>
+  </si>
+  <si>
+    <t>Suyog Talathi</t>
+  </si>
+  <si>
+    <t>testautocomponent_628539</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>testautocomponent_166931</t>
+  </si>
+  <si>
+    <t>testautocomponent_3973701</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>testautocomponent_643036</t>
+  </si>
+  <si>
+    <t>testautocomponent_912424</t>
+  </si>
+  <si>
+    <t>testautocomponent_961785</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -307,10 +337,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A36E2ED-4772-47F9-B35C-8CB5C4409702}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -846,10 +877,162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8818ED2-DC59-4EB8-A9A5-6F4594129690}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>320</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3">
+        <v>43209.541562500002</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>319</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43209.521828703706</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43209.537789351853</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>318</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43209.490682870368</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>317</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43209.484513888892</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>316</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43209.420578703706</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43209.454317129632</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>315</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43209.416608796295</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
@@ -935,8 +1118,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA5F027-FF63-48EB-B373-A7B956E95C47}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1026,8 +1209,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258EB639-EA61-477D-98E2-6A869BB70443}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1149,8 +1332,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE145A48-B877-4FE4-AFD8-C169CA3698A6}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1302,8 +1485,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10CCCAB-3C83-4826-8754-CDF22F24FE6F}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1500,8 +1683,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4354C65F-217B-4E18-B9F8-2FDD8991002A}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1598,8 +1781,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B04FFD-6DE8-406C-BAD2-FF88C9BE92CC}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[ST 23 April 2018] Updated code for Login to app, Create new ds flow, Visualize page
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Visualize" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>testautocomponent_961785</t>
+  </si>
+  <si>
+    <t>testautocomponent_379767</t>
   </si>
 </sst>
 </file>
@@ -658,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -878,9 +881,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -896,10 +899,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
         <v>80</v>
@@ -908,7 +911,7 @@
         <v>81</v>
       </c>
       <c r="E1" s="3">
-        <v>43209.541562500002</v>
+        <v>43210.471770833334</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" t="s">
@@ -917,10 +920,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>80</v>
@@ -929,21 +932,19 @@
         <v>81</v>
       </c>
       <c r="E2" s="3">
-        <v>43209.521828703706</v>
-      </c>
-      <c r="F2" s="3">
-        <v>43209.537789351853</v>
-      </c>
+        <v>43209.541562500002</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
@@ -952,19 +953,21 @@
         <v>81</v>
       </c>
       <c r="E3" s="3">
-        <v>43209.490682870368</v>
-      </c>
-      <c r="F3" s="3"/>
+        <v>43209.521828703706</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43209.537789351853</v>
+      </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>80</v>
@@ -973,7 +976,7 @@
         <v>81</v>
       </c>
       <c r="E4" s="3">
-        <v>43209.484513888892</v>
+        <v>43209.490682870368</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" t="s">
@@ -982,10 +985,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>80</v>
@@ -994,21 +997,19 @@
         <v>81</v>
       </c>
       <c r="E5" s="3">
-        <v>43209.420578703706</v>
-      </c>
-      <c r="F5" s="3">
-        <v>43209.454317129632</v>
-      </c>
+        <v>43209.484513888892</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>80</v>
@@ -1017,9 +1018,32 @@
         <v>81</v>
       </c>
       <c r="E6" s="3">
+        <v>43209.420578703706</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43209.454317129632</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>315</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="3">
         <v>43209.416608796295</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[AA | 30/04/2018] : Run Configurtion Changes , API ML Model changes
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_Local\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4733DA-7B0A-4FC4-AAA5-2E29623BFFAD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TagsData" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="ExistingRunConfig_Data" sheetId="3" r:id="rId1"/>
+    <sheet name="TagsData" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Suyog Talathi</t>
   </si>
@@ -34,12 +36,75 @@
   </si>
   <si>
     <t>TestShortDescription_8837...</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Level 6</t>
+  </si>
+  <si>
+    <t>Level 7</t>
+  </si>
+  <si>
+    <t>Level 8</t>
+  </si>
+  <si>
+    <t>Level 9</t>
+  </si>
+  <si>
+    <t>Level 10</t>
+  </si>
+  <si>
+    <t>Level 11</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Level 12</t>
+  </si>
+  <si>
+    <t>Level 13</t>
+  </si>
+  <si>
+    <t>Level 14</t>
+  </si>
+  <si>
+    <t>Level 15</t>
+  </si>
+  <si>
+    <t>Level 16</t>
+  </si>
+  <si>
+    <t>Level 17</t>
+  </si>
+  <si>
+    <t>Level 18</t>
+  </si>
+  <si>
+    <t>Level 19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,28 +416,411 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C73961-1F30-4D94-AFB2-B131E11BA7AB}">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>43217.649826388886</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>99</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -381,7 +829,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>43217.649826388886</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[ST - 3 May 2018 ] Updated code for Querying page, Connectors
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_Local\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4733DA-7B0A-4FC4-AAA5-2E29623BFFAD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
-    <sheet name="ExistingRunConfig_Data" sheetId="3" r:id="rId1"/>
-    <sheet name="TagsData" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Visualize" sheetId="4" r:id="rId1"/>
+    <sheet name="ExistingRunConfig_Data" sheetId="3" r:id="rId2"/>
+    <sheet name="TagsData" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,10 +416,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C73961-1F30-4D94-AFB2-B131E11BA7AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -828,8 +840,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -858,8 +870,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[AA | 11/05/2018] : Chnages for TC mapping
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_Local\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23190F42-CCA9-4EBB-963F-CB13B952D20C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{BE9109A2-E69C-4DD2-A164-258255FC9FA6}"/>
   </bookViews>
   <sheets>
-    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId1"/>
+    <sheet name="ExistingRunConfig_Data" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +25,112 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Level 6</t>
+  </si>
+  <si>
+    <t>Level 7</t>
+  </si>
+  <si>
+    <t>Level 8</t>
+  </si>
+  <si>
+    <t>Level 9</t>
+  </si>
+  <si>
+    <t>Level 10</t>
+  </si>
+  <si>
+    <t>Level 11</t>
+  </si>
+  <si>
+    <t>Level 12</t>
+  </si>
+  <si>
+    <t>Level 13</t>
+  </si>
+  <si>
+    <t>Level 14</t>
+  </si>
+  <si>
+    <t>Level 15</t>
+  </si>
+  <si>
+    <t>Level 16</t>
+  </si>
+  <si>
+    <t>Level 17</t>
+  </si>
+  <si>
+    <t>Level 18</t>
+  </si>
+  <si>
+    <t>Level 19</t>
+  </si>
+  <si>
+    <t>Level 20</t>
+  </si>
+  <si>
+    <t>Level 21</t>
+  </si>
+  <si>
+    <t>Level 22</t>
+  </si>
+  <si>
+    <t>Level 23</t>
+  </si>
+  <si>
+    <t>Level 24</t>
+  </si>
+  <si>
+    <t>Level 25</t>
+  </si>
+  <si>
+    <t>Level 26</t>
+  </si>
+  <si>
+    <t>Level 27</t>
+  </si>
+  <si>
+    <t>Level 28</t>
+  </si>
+  <si>
+    <t>Level 29</t>
+  </si>
+  <si>
+    <t>Level 30</t>
+  </si>
+  <si>
+    <t>Level 31</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,7 +196,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -103,7 +208,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -120,9 +225,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -150,14 +255,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -185,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,19 +475,660 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33EDDFB-C488-4350-B677-C7FD671FD849}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>99</v>
+      </c>
+      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>99</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BA3265-BDAF-40A9-9347-9751FB04A713}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[ST - 11-05-2018 Updated code for mapping For Catalog page, visualize page, Login poage, project page, developer page]
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_Local\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
-    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Process_SortNode" sheetId="3" r:id="rId1"/>
+    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -22,6 +23,137 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+  <si>
+    <t>AAVESH</t>
+  </si>
+  <si>
+    <t>RESEARCH</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>8 years</t>
+  </si>
+  <si>
+    <t>DAVID</t>
+  </si>
+  <si>
+    <t>AMAN</t>
+  </si>
+  <si>
+    <t>Automation Anywhere</t>
+  </si>
+  <si>
+    <t>4 years</t>
+  </si>
+  <si>
+    <t>GIRISH</t>
+  </si>
+  <si>
+    <t>AMOL</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>6 years</t>
+  </si>
+  <si>
+    <t>UiPath</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>MARTIN</t>
+  </si>
+  <si>
+    <t>12 years</t>
+  </si>
+  <si>
+    <t>NOOO</t>
+  </si>
+  <si>
+    <t>MILLER</t>
+  </si>
+  <si>
+    <t>ACCOUNTING</t>
+  </si>
+  <si>
+    <t>Blue Prism</t>
+  </si>
+  <si>
+    <t>13 years</t>
+  </si>
+  <si>
+    <t>NISHA</t>
+  </si>
+  <si>
+    <t>RPA</t>
+  </si>
+  <si>
+    <t>11 years</t>
+  </si>
+  <si>
+    <t>TEJAS</t>
+  </si>
+  <si>
+    <t>SACHIN</t>
+  </si>
+  <si>
+    <t>20 years</t>
+  </si>
+  <si>
+    <t>MANU</t>
+  </si>
+  <si>
+    <t>SANGEETA</t>
+  </si>
+  <si>
+    <t>10 years</t>
+  </si>
+  <si>
+    <t>SAURABH</t>
+  </si>
+  <si>
+    <t>SANTOSH</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>9 years</t>
+  </si>
+  <si>
+    <t>NONAME</t>
+  </si>
+  <si>
+    <t>SCOTT</t>
+  </si>
+  <si>
+    <t>14 years</t>
+  </si>
+  <si>
+    <t>LOL</t>
+  </si>
+  <si>
+    <t>SUYOG</t>
+  </si>
+  <si>
+    <t>7 years</t>
+  </si>
+  <si>
+    <t>ayusH</t>
+  </si>
+  <si>
+    <t>NONAA</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,12 +469,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -357,4 +750,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[AA | 11/05/2018] : Mapping of TC's for reporting
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23190F42-CCA9-4EBB-963F-CB13B952D20C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AB2A74-12E7-4FA7-BED7-0D0B096AE014}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{BE9109A2-E69C-4DD2-A164-258255FC9FA6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>Level 1</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>Level 31</t>
+  </si>
+  <si>
+    <t>Level 32</t>
+  </si>
+  <si>
+    <t>Level 33</t>
+  </si>
+  <si>
+    <t>Level 34</t>
+  </si>
+  <si>
+    <t>Level 35</t>
+  </si>
+  <si>
+    <t>Level 36</t>
+  </si>
+  <si>
+    <t>Level 37</t>
   </si>
 </sst>
 </file>
@@ -476,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33EDDFB-C488-4350-B677-C7FD671FD849}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -787,16 +805,16 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
         <v>3</v>
@@ -810,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -827,16 +845,16 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
         <v>3</v>
@@ -850,10 +868,10 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -870,13 +888,13 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>3</v>
@@ -890,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -907,16 +925,16 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -924,19 +942,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
         <v>3</v>
@@ -944,13 +962,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -964,19 +982,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>3</v>
@@ -984,19 +1002,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F26" t="s">
         <v>3</v>
@@ -1004,19 +1022,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>3</v>
@@ -1024,19 +1042,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s">
         <v>3</v>
@@ -1047,13 +1065,13 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E29">
         <v>7</v>
@@ -1067,16 +1085,16 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
         <v>3</v>
@@ -1087,16 +1105,16 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -1107,18 +1125,138 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[AA | 14/05/2018] : Test Case Changes
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0D0848-3878-4DEF-939A-88B95F90B0D7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Process_SortNode" sheetId="3" r:id="rId1"/>
-    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Process_FeaturesNode" sheetId="4" r:id="rId1"/>
+    <sheet name="Process_SortNode" sheetId="3" r:id="rId2"/>
+    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="55">
   <si>
     <t>AAVESH</t>
   </si>
@@ -152,12 +154,51 @@
   </si>
   <si>
     <t>NONAA</t>
+  </si>
+  <si>
+    <t>AMANAutomation Anywhere</t>
+  </si>
+  <si>
+    <t>GIRISHUiPath</t>
+  </si>
+  <si>
+    <t>AMOLAutomation Anywhere</t>
+  </si>
+  <si>
+    <t>SUYOGBlue Prism</t>
+  </si>
+  <si>
+    <t>AAVESHDevelopment</t>
+  </si>
+  <si>
+    <t>SANTOSHSelenium</t>
+  </si>
+  <si>
+    <t>SANGEETAUiPath</t>
+  </si>
+  <si>
+    <t>NISHARPA</t>
+  </si>
+  <si>
+    <t>MARTINAutomation Anywhere</t>
+  </si>
+  <si>
+    <t>MILLERBlue Prism</t>
+  </si>
+  <si>
+    <t>SCOTTUiPath</t>
+  </si>
+  <si>
+    <t>SACHINRPA</t>
+  </si>
+  <si>
+    <t>ayusHSelenium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,10 +509,322 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A6D198-329B-474B-B504-241EA8C2DA44}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -740,8 +1093,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -752,8 +1105,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[ST- 22 May 18 : Updated code for reporting changes]
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0D0848-3878-4DEF-939A-88B95F90B0D7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Process_FeaturesNode" sheetId="4" r:id="rId1"/>
-    <sheet name="Process_SortNode" sheetId="3" r:id="rId2"/>
-    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="DeveloperTabData" sheetId="5" r:id="rId1"/>
+    <sheet name="Process_FeaturesNode" sheetId="4" r:id="rId2"/>
+    <sheet name="Process_SortNode" sheetId="3" r:id="rId3"/>
+    <sheet name="ProcessLookUpNode" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
   <si>
     <t>AAVESH</t>
   </si>
@@ -193,12 +193,39 @@
   </si>
   <si>
     <t>ayusHSelenium</t>
+  </si>
+  <si>
+    <t>testautocomponent_391453</t>
+  </si>
+  <si>
+    <t>Shell Script</t>
+  </si>
+  <si>
+    <t>Suyog Talathi</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>testcomponenr</t>
+  </si>
+  <si>
+    <t>Girish Agrawal</t>
+  </si>
+  <si>
+    <t>new_component</t>
+  </si>
+  <si>
+    <t>Aman Garg</t>
+  </si>
+  <si>
+    <t>Updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,8 +255,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,310 +537,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A6D198-329B-474B-B504-241EA8C2DA44}">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
+      <c r="A1">
+        <v>340</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="E1" s="1">
+        <v>43242.649317129632</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>101</v>
+      <c r="A2">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43176.509305555555</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>102</v>
+      <c r="A3">
+        <v>239</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43132.804606481484</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43176.508796296293</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
-        <v>103</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>104</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>105</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7">
-        <v>106</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <v>107</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>108</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>109</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11">
-        <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12">
-        <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13">
-        <v>112</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +613,319 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1093,8 +1197,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1105,8 +1209,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[AG: 24/05- updated code for flow, visualize and compare CSV file]
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DeveloperTabData" sheetId="5" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -928,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
[ST- Updated code For Fixes]
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="105"/>
   </bookViews>
   <sheets>
     <sheet name="DeveloperTabData" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="66">
   <si>
     <t>AAVESH</t>
   </si>
@@ -220,12 +220,18 @@
   </si>
   <si>
     <t>Updated</t>
+  </si>
+  <si>
+    <t>testautocomponent_560547</t>
+  </si>
+  <si>
+    <t>testautocomponent_731106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -538,18 +544,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>56</v>
@@ -558,7 +564,7 @@
         <v>57</v>
       </c>
       <c r="E1" s="1">
-        <v>43242.649317129632</v>
+        <v>43245.022847222222</v>
       </c>
       <c r="G1" t="s">
         <v>58</v>
@@ -566,19 +572,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>287</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" s="1">
-        <v>43176.509305555555</v>
+        <v>43244.94027777778</v>
       </c>
       <c r="G2" t="s">
         <v>58</v>
@@ -586,24 +592,66 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>239</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43242.649317129632</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>287</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43176.509305555555</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>239</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E5" s="1">
         <v>43132.804606481484</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F5" s="1">
         <v>43176.508796296293</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -928,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
[ST : 28 may 2018 : Updated code for summary report : Inprogress]
</commit_message>
<xml_diff>
--- a/TableCompare/ActualDataFile.xlsx
+++ b/TableCompare/ActualDataFile.xlsx
@@ -225,7 +225,7 @@
     <t>testautocomponent_560547</t>
   </si>
   <si>
-    <t>testautocomponent_731106</t>
+    <t>testautocomponent_709005</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>345</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
         <v>65</v>
@@ -564,7 +564,7 @@
         <v>57</v>
       </c>
       <c r="E1" s="1">
-        <v>43245.022847222222</v>
+        <v>43245.707569444443</v>
       </c>
       <c r="G1" t="s">
         <v>58</v>

</xml_diff>